<commit_message>
Updated funds with more tabs
</commit_message>
<xml_diff>
--- a/parameters/invmt_portfolio_mapper.xlsx
+++ b/parameters/invmt_portfolio_mapper.xlsx
@@ -170,9 +170,6 @@
     <t>COUNTRY</t>
   </si>
   <si>
-    <t>TRADELOCALCURRENCY</t>
-  </si>
-  <si>
     <t>CREDITRATINGS</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>LOCALCURR</t>
   </si>
 </sst>
 </file>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -766,13 +766,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -820,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -836,7 +836,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -844,7 +844,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -852,7 +852,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -863,21 +863,21 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -885,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -893,7 +893,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -901,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -909,10 +909,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>15</v>
@@ -938,7 +938,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="3"/>
     </row>
@@ -993,7 +993,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="7"/>
     </row>
@@ -1002,7 +1002,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>33</v>
@@ -1021,7 +1021,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3">

</xml_diff>